<commit_message>
new names, path creation adaptation for executable
</commit_message>
<xml_diff>
--- a/stimuli/conditions.xlsx
+++ b/stimuli/conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd04e49f116cdb8a/PhD/exp_dualtask/stimuli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="8_{7C71BDAE-B2CB-4516-9F1B-5254DB8750DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C1DB9A8-2370-4EED-AF7C-AA576FDC7374}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{7C71BDAE-B2CB-4516-9F1B-5254DB8750DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D9AD472-A116-4631-868A-D68073B36E15}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="2424" windowWidth="21600" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -857,6 +857,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1159,12 +1163,12 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>

</xml_diff>